<commit_message>
feat(customer-order): update file template
</commit_message>
<xml_diff>
--- a/Programming/WebFrontEnd/public/files/template-customer-order.xlsx
+++ b/Programming/WebFrontEnd/public/files/template-customer-order.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">No</t>
   </si>
   <si>
-    <t xml:space="preserve">Sub Budget</t>
+    <t xml:space="preserve">Sub Budget Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub Budget Name</t>
   </si>
   <si>
     <t xml:space="preserve">Value</t>
@@ -328,16 +331,16 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="114" zoomScaleNormal="114" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="13.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="27.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="13.88"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -352,6 +355,9 @@
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -359,7 +365,10 @@
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>